<commit_message>
Namen gefixt in Feedback bestand
</commit_message>
<xml_diff>
--- a/Feedback PAC.xlsx
+++ b/Feedback PAC.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stichtingfontys.sharepoint.com/sites/Project3990/Gedeelde documenten/General/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c1aa17d595c3374/School/Jaar 2/Project 5/Project_5/Project_5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="325" documentId="13_ncr:1_{D3268C1E-1F1E-4E42-AE04-06F5504078FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C4AB2DA-1583-47B0-A1BC-1061E8320944}"/>
+  <xr:revisionPtr revIDLastSave="330" documentId="13_ncr:1_{D3268C1E-1F1E-4E42-AE04-06F5504078FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC2B8480-1F58-453E-AD87-8612758BE359}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="803" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="803" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="voor dylan" sheetId="55" r:id="rId1"/>
-    <sheet name="voor lars" sheetId="54" r:id="rId2"/>
-    <sheet name="voor serve" sheetId="53" r:id="rId3"/>
-    <sheet name="voor richard" sheetId="52" r:id="rId4"/>
-    <sheet name="voor lieke" sheetId="47" r:id="rId5"/>
-    <sheet name="Feedback onderwerpen" sheetId="30" r:id="rId6"/>
+    <sheet name="Voor Bram" sheetId="55" r:id="rId1"/>
+    <sheet name="Voor Lars" sheetId="54" r:id="rId2"/>
+    <sheet name="Voor Floor" sheetId="53" r:id="rId3"/>
+    <sheet name="Voor Jinne" sheetId="52" r:id="rId4"/>
+    <sheet name="Feedback onderwerpen" sheetId="30" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="123">
   <si>
     <t>Feedback Format</t>
   </si>
@@ -510,7 +509,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -827,16 +826,40 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -851,49 +874,25 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1182,49 +1181,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5192037A-3EA1-4D22-9A23-B1FE1A814A0A}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="F13" sqref="F13:G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
-    <col min="2" max="2" width="100.7109375" customWidth="1"/>
-    <col min="3" max="3" width="70.7109375" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" customWidth="1"/>
-    <col min="6" max="6" width="100.7109375" customWidth="1"/>
-    <col min="7" max="7" width="70.7109375" customWidth="1"/>
-    <col min="9" max="9" width="28.28515625" customWidth="1"/>
-    <col min="10" max="10" width="100.7109375" customWidth="1"/>
-    <col min="11" max="11" width="70.7109375" customWidth="1"/>
-    <col min="13" max="13" width="28.28515625" customWidth="1"/>
-    <col min="14" max="14" width="100.7109375" customWidth="1"/>
-    <col min="15" max="15" width="70.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" customWidth="1"/>
+    <col min="3" max="3" width="70.6640625" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="100.6640625" customWidth="1"/>
+    <col min="7" max="7" width="70.6640625" customWidth="1"/>
+    <col min="9" max="9" width="28.33203125" customWidth="1"/>
+    <col min="10" max="10" width="100.6640625" customWidth="1"/>
+    <col min="11" max="11" width="70.6640625" customWidth="1"/>
+    <col min="13" max="13" width="28.33203125" customWidth="1"/>
+    <col min="14" max="14" width="100.6640625" customWidth="1"/>
+    <col min="15" max="15" width="70.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="28.35" customHeight="1">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:15" ht="28.35" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="46"/>
-      <c r="E1" s="45" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="30"/>
+      <c r="E1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="45"/>
-      <c r="G1" s="46"/>
-      <c r="I1" s="45" t="s">
+      <c r="F1" s="29"/>
+      <c r="G1" s="30"/>
+      <c r="I1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="45"/>
-      <c r="K1" s="46"/>
-      <c r="M1" s="45" t="s">
+      <c r="J1" s="29"/>
+      <c r="K1" s="30"/>
+      <c r="M1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="N1" s="45"/>
-      <c r="O1" s="46"/>
-    </row>
-    <row r="2" spans="1:15" ht="20.25">
+      <c r="N1" s="29"/>
+      <c r="O1" s="30"/>
+    </row>
+    <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
@@ -1254,7 +1253,7 @@
       </c>
       <c r="O2" s="24"/>
     </row>
-    <row r="3" spans="1:15" ht="20.25">
+    <row r="3" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="15" t="s">
         <v>3</v>
       </c>
@@ -1284,7 +1283,7 @@
       </c>
       <c r="O3" s="24"/>
     </row>
-    <row r="4" spans="1:15" ht="20.25">
+    <row r="4" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A4" s="15" t="s">
         <v>5</v>
       </c>
@@ -1314,7 +1313,7 @@
       </c>
       <c r="O4" s="24"/>
     </row>
-    <row r="5" spans="1:15" ht="20.25">
+    <row r="5" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
         <v>10</v>
       </c>
@@ -1344,7 +1343,7 @@
       </c>
       <c r="O5" s="24"/>
     </row>
-    <row r="6" spans="1:15" s="17" customFormat="1" ht="20.25">
+    <row r="6" spans="1:15" s="17" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A6" s="16" t="s">
         <v>12</v>
       </c>
@@ -1374,7 +1373,7 @@
       </c>
       <c r="O6" s="26"/>
     </row>
-    <row r="7" spans="1:15" ht="20.25">
+    <row r="7" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
@@ -1404,413 +1403,413 @@
       </c>
       <c r="O7" s="24"/>
     </row>
-    <row r="8" spans="1:15" ht="15.6" customHeight="1">
-      <c r="A8" s="37" t="s">
+    <row r="8" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="38"/>
-      <c r="E8" s="37" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="28"/>
+      <c r="E8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="38"/>
-      <c r="I8" s="37" t="s">
+      <c r="F8" s="27"/>
+      <c r="G8" s="28"/>
+      <c r="I8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="37"/>
-      <c r="K8" s="38"/>
-      <c r="M8" s="37" t="s">
+      <c r="J8" s="27"/>
+      <c r="K8" s="28"/>
+      <c r="M8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="37"/>
-      <c r="O8" s="38"/>
-    </row>
-    <row r="9" spans="1:15" ht="23.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="44"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="44"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="44"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="43"/>
-      <c r="O9" s="44"/>
-    </row>
-    <row r="10" spans="1:15" ht="105.75" customHeight="1">
+      <c r="N8" s="27"/>
+      <c r="O8" s="28"/>
+    </row>
+    <row r="9" spans="1:15" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="32"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="32"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="32"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="32"/>
+    </row>
+    <row r="10" spans="1:15" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="42"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="22"/>
       <c r="E10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="41" t="s">
+      <c r="F10" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="42"/>
+      <c r="G10" s="34"/>
       <c r="H10" s="22"/>
       <c r="I10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="41" t="s">
+      <c r="J10" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="42"/>
+      <c r="K10" s="34"/>
       <c r="L10" s="22"/>
       <c r="M10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="N10" s="41" t="s">
+      <c r="N10" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="O10" s="42"/>
-    </row>
-    <row r="11" spans="1:15" ht="134.25" customHeight="1">
+      <c r="O10" s="34"/>
+    </row>
+    <row r="11" spans="1:15" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="30"/>
+      <c r="C11" s="36"/>
       <c r="D11" s="22"/>
       <c r="E11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="30"/>
+      <c r="G11" s="36"/>
       <c r="H11" s="22"/>
       <c r="I11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="29" t="s">
+      <c r="J11" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="K11" s="30"/>
+      <c r="K11" s="36"/>
       <c r="L11" s="22"/>
       <c r="M11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="29" t="s">
+      <c r="N11" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="O11" s="30"/>
-    </row>
-    <row r="12" spans="1:15" ht="23.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="40"/>
+      <c r="O11" s="36"/>
+    </row>
+    <row r="12" spans="1:15" ht="22.8" x14ac:dyDescent="0.25">
+      <c r="A12" s="37"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="22"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="40"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="38"/>
       <c r="H12" s="22"/>
       <c r="I12" s="21"/>
-      <c r="J12" s="39" t="s">
+      <c r="J12" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="40"/>
+      <c r="K12" s="38"/>
       <c r="L12" s="22"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="40"/>
-    </row>
-    <row r="13" spans="1:15" ht="96.75" customHeight="1">
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="38"/>
+    </row>
+    <row r="13" spans="1:15" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="42"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="22"/>
       <c r="E13" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="41" t="s">
+      <c r="F13" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="42"/>
+      <c r="G13" s="34"/>
       <c r="H13" s="22"/>
       <c r="I13" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="J13" s="41" t="s">
+      <c r="J13" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="K13" s="42"/>
+      <c r="K13" s="34"/>
       <c r="L13" s="22"/>
       <c r="M13" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="N13" s="41" t="s">
+      <c r="N13" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="O13" s="42"/>
-    </row>
-    <row r="14" spans="1:15" ht="62.25" customHeight="1">
+      <c r="O13" s="34"/>
+    </row>
+    <row r="14" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="30"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="22"/>
       <c r="E14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="30"/>
+      <c r="G14" s="36"/>
       <c r="H14" s="22"/>
       <c r="I14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="29" t="s">
+      <c r="J14" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="K14" s="30"/>
+      <c r="K14" s="36"/>
       <c r="L14" s="22"/>
       <c r="M14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="N14" s="29" t="s">
+      <c r="N14" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="O14" s="30"/>
-    </row>
-    <row r="15" spans="1:15" ht="23.25">
-      <c r="A15" s="39"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="40"/>
+      <c r="O14" s="36"/>
+    </row>
+    <row r="15" spans="1:15" ht="22.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="38"/>
       <c r="D15" s="22"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="40"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="38"/>
       <c r="H15" s="22"/>
       <c r="I15" s="21"/>
-      <c r="J15" s="39" t="s">
+      <c r="J15" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="40"/>
+      <c r="K15" s="38"/>
       <c r="L15" s="22"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
-      <c r="O15" s="40"/>
-    </row>
-    <row r="16" spans="1:15" ht="75.75" customHeight="1">
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="38"/>
+    </row>
+    <row r="16" spans="1:15" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="42"/>
+      <c r="C16" s="34"/>
       <c r="D16" s="22"/>
       <c r="E16" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="41" t="s">
+      <c r="F16" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="42"/>
+      <c r="G16" s="34"/>
       <c r="H16" s="22"/>
       <c r="I16" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="41" t="s">
+      <c r="J16" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="K16" s="42"/>
+      <c r="K16" s="34"/>
       <c r="L16" s="22"/>
       <c r="M16" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="N16" s="41" t="s">
+      <c r="N16" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="O16" s="42"/>
-    </row>
-    <row r="17" spans="1:15" ht="92.25" customHeight="1">
+      <c r="O16" s="34"/>
+    </row>
+    <row r="17" spans="1:15" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="30"/>
+      <c r="C17" s="36"/>
       <c r="D17" s="22"/>
       <c r="E17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="29" t="s">
+      <c r="F17" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="30"/>
+      <c r="G17" s="36"/>
       <c r="H17" s="22"/>
       <c r="I17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="J17" s="29" t="s">
+      <c r="J17" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="K17" s="30"/>
+      <c r="K17" s="36"/>
       <c r="L17" s="22"/>
       <c r="M17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="N17" s="29" t="s">
+      <c r="N17" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="O17" s="30"/>
-    </row>
-    <row r="21" spans="1:15" ht="27.75">
-      <c r="A21" s="33" t="s">
+      <c r="O17" s="36"/>
+    </row>
+    <row r="21" spans="1:15" ht="28.2" x14ac:dyDescent="0.5">
+      <c r="A21" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="34"/>
-    </row>
-    <row r="22" spans="1:15" ht="20.25">
+      <c r="B21" s="41"/>
+      <c r="C21" s="42"/>
+    </row>
+    <row r="22" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A22" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="49"/>
-    </row>
-    <row r="23" spans="1:15" ht="20.25">
+      <c r="C22" s="44"/>
+    </row>
+    <row r="23" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A23" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="49"/>
-    </row>
-    <row r="24" spans="1:15" ht="20.25">
+      <c r="C23" s="44"/>
+    </row>
+    <row r="24" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A24" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="50" t="s">
+      <c r="B24" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="49"/>
-    </row>
-    <row r="25" spans="1:15" s="17" customFormat="1" ht="20.25">
+      <c r="C24" s="44"/>
+    </row>
+    <row r="25" spans="1:15" s="17" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A25" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="35">
+      <c r="B25" s="46">
         <v>45392</v>
       </c>
-      <c r="C25" s="36"/>
-    </row>
-    <row r="26" spans="1:15" ht="20.25">
+      <c r="C25" s="47"/>
+    </row>
+    <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A26" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="48" t="s">
+      <c r="B26" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="49"/>
-    </row>
-    <row r="27" spans="1:15" ht="15.75">
-      <c r="A27" s="37" t="s">
+      <c r="C26" s="44"/>
+    </row>
+    <row r="27" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="38"/>
-    </row>
-    <row r="28" spans="1:15" ht="23.25">
-      <c r="A28" s="31" t="s">
+      <c r="B27" s="27"/>
+      <c r="C27" s="28"/>
+    </row>
+    <row r="28" spans="1:15" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A28" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="32"/>
-    </row>
-    <row r="29" spans="1:15" ht="101.25" customHeight="1">
+      <c r="B28" s="39"/>
+      <c r="C28" s="40"/>
+    </row>
+    <row r="29" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="28"/>
-    </row>
-    <row r="30" spans="1:15" ht="110.25" customHeight="1">
+      <c r="C29" s="49"/>
+    </row>
+    <row r="30" spans="1:15" ht="110.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="30"/>
-    </row>
-    <row r="31" spans="1:15" ht="23.25">
-      <c r="A31" s="31" t="s">
+      <c r="C30" s="36"/>
+    </row>
+    <row r="31" spans="1:15" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A31" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="32"/>
-    </row>
-    <row r="32" spans="1:15" ht="99.75" customHeight="1">
+      <c r="B31" s="39"/>
+      <c r="C31" s="40"/>
+    </row>
+    <row r="32" spans="1:15" ht="99.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="28"/>
-    </row>
-    <row r="33" spans="1:3" ht="56.25" customHeight="1">
+      <c r="C32" s="49"/>
+    </row>
+    <row r="33" spans="1:3" ht="56.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="30"/>
-    </row>
-    <row r="34" spans="1:3" ht="23.25">
-      <c r="A34" s="31" t="s">
+      <c r="C33" s="36"/>
+    </row>
+    <row r="34" spans="1:3" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A34" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="32"/>
-    </row>
-    <row r="35" spans="1:3" ht="94.5" customHeight="1">
+      <c r="B34" s="39"/>
+      <c r="C34" s="40"/>
+    </row>
+    <row r="35" spans="1:3" ht="94.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="28"/>
-    </row>
-    <row r="36" spans="1:3" ht="72" customHeight="1">
+      <c r="C35" s="49"/>
+    </row>
+    <row r="36" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="29" t="s">
+      <c r="B36" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="30"/>
-    </row>
-    <row r="38" spans="1:3" ht="15.75">
+      <c r="C36" s="36"/>
+    </row>
+    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>48</v>
       </c>
@@ -1818,46 +1817,14 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="A34:C34"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="F17:G17"/>
@@ -1870,14 +1837,46 @@
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="A27:C27"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="M1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1891,45 +1890,45 @@
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
-    <col min="2" max="2" width="100.7109375" customWidth="1"/>
-    <col min="3" max="3" width="70.7109375" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" customWidth="1"/>
-    <col min="6" max="6" width="100.7109375" customWidth="1"/>
-    <col min="7" max="7" width="70.7109375" customWidth="1"/>
-    <col min="9" max="9" width="28.28515625" customWidth="1"/>
-    <col min="10" max="10" width="100.7109375" customWidth="1"/>
-    <col min="11" max="11" width="70.7109375" customWidth="1"/>
-    <col min="13" max="13" width="28.28515625" customWidth="1"/>
-    <col min="14" max="14" width="100.7109375" customWidth="1"/>
-    <col min="15" max="15" width="70.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" customWidth="1"/>
+    <col min="3" max="3" width="70.6640625" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="100.6640625" customWidth="1"/>
+    <col min="7" max="7" width="70.6640625" customWidth="1"/>
+    <col min="9" max="9" width="28.33203125" customWidth="1"/>
+    <col min="10" max="10" width="100.6640625" customWidth="1"/>
+    <col min="11" max="11" width="70.6640625" customWidth="1"/>
+    <col min="13" max="13" width="28.33203125" customWidth="1"/>
+    <col min="14" max="14" width="100.6640625" customWidth="1"/>
+    <col min="15" max="15" width="70.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="28.35" customHeight="1">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:15" ht="28.35" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="46"/>
-      <c r="E1" s="45" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="30"/>
+      <c r="E1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="45"/>
-      <c r="G1" s="46"/>
-      <c r="I1" s="45" t="s">
+      <c r="F1" s="29"/>
+      <c r="G1" s="30"/>
+      <c r="I1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="45"/>
-      <c r="K1" s="46"/>
-      <c r="M1" s="45" t="s">
+      <c r="J1" s="29"/>
+      <c r="K1" s="30"/>
+      <c r="M1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="N1" s="45"/>
-      <c r="O1" s="46"/>
-    </row>
-    <row r="2" spans="1:15" ht="20.25">
+      <c r="N1" s="29"/>
+      <c r="O1" s="30"/>
+    </row>
+    <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
@@ -1959,7 +1958,7 @@
       </c>
       <c r="O2" s="24"/>
     </row>
-    <row r="3" spans="1:15" ht="20.25">
+    <row r="3" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="15" t="s">
         <v>3</v>
       </c>
@@ -1989,7 +1988,7 @@
       </c>
       <c r="O3" s="24"/>
     </row>
-    <row r="4" spans="1:15" ht="20.25">
+    <row r="4" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A4" s="15" t="s">
         <v>5</v>
       </c>
@@ -2019,7 +2018,7 @@
       </c>
       <c r="O4" s="24"/>
     </row>
-    <row r="5" spans="1:15" ht="20.25">
+    <row r="5" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
         <v>10</v>
       </c>
@@ -2049,7 +2048,7 @@
       </c>
       <c r="O5" s="24"/>
     </row>
-    <row r="6" spans="1:15" s="17" customFormat="1" ht="20.25">
+    <row r="6" spans="1:15" s="17" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A6" s="16" t="s">
         <v>12</v>
       </c>
@@ -2079,7 +2078,7 @@
       </c>
       <c r="O6" s="26"/>
     </row>
-    <row r="7" spans="1:15" ht="20.25">
+    <row r="7" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
@@ -2109,458 +2108,426 @@
       </c>
       <c r="O7" s="24"/>
     </row>
-    <row r="8" spans="1:15" ht="15.6" customHeight="1">
-      <c r="A8" s="37" t="s">
+    <row r="8" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="38"/>
-      <c r="E8" s="37" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="28"/>
+      <c r="E8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="38"/>
-      <c r="I8" s="37" t="s">
+      <c r="F8" s="27"/>
+      <c r="G8" s="28"/>
+      <c r="I8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="37"/>
-      <c r="K8" s="38"/>
-      <c r="M8" s="37" t="s">
+      <c r="J8" s="27"/>
+      <c r="K8" s="28"/>
+      <c r="M8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="37"/>
-      <c r="O8" s="38"/>
-    </row>
-    <row r="9" spans="1:15" ht="23.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="44"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="44"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="44"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="43"/>
-      <c r="O9" s="44"/>
-    </row>
-    <row r="10" spans="1:15" ht="105.75" customHeight="1">
+      <c r="N8" s="27"/>
+      <c r="O8" s="28"/>
+    </row>
+    <row r="9" spans="1:15" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="32"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="32"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="32"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="32"/>
+    </row>
+    <row r="10" spans="1:15" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="42"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="22"/>
       <c r="E10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="41" t="s">
+      <c r="F10" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="42"/>
+      <c r="G10" s="34"/>
       <c r="H10" s="22"/>
       <c r="I10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="41" t="s">
+      <c r="J10" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="42"/>
+      <c r="K10" s="34"/>
       <c r="L10" s="22"/>
       <c r="M10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="N10" s="41" t="s">
+      <c r="N10" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="O10" s="42"/>
-    </row>
-    <row r="11" spans="1:15" ht="134.25" customHeight="1">
+      <c r="O10" s="34"/>
+    </row>
+    <row r="11" spans="1:15" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="30"/>
+      <c r="C11" s="36"/>
       <c r="D11" s="22"/>
       <c r="E11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="30"/>
+      <c r="G11" s="36"/>
       <c r="H11" s="22"/>
       <c r="I11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="29" t="s">
+      <c r="J11" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="K11" s="30"/>
+      <c r="K11" s="36"/>
       <c r="L11" s="22"/>
       <c r="M11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="29" t="s">
+      <c r="N11" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="O11" s="30"/>
-    </row>
-    <row r="12" spans="1:15" ht="23.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="40"/>
+      <c r="O11" s="36"/>
+    </row>
+    <row r="12" spans="1:15" ht="22.8" x14ac:dyDescent="0.25">
+      <c r="A12" s="37"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="22"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="40"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="38"/>
       <c r="H12" s="22"/>
       <c r="I12" s="21"/>
-      <c r="J12" s="39" t="s">
+      <c r="J12" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="40"/>
+      <c r="K12" s="38"/>
       <c r="L12" s="22"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="40"/>
-    </row>
-    <row r="13" spans="1:15" ht="96.75" customHeight="1">
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="38"/>
+    </row>
+    <row r="13" spans="1:15" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="42"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="22"/>
       <c r="E13" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="41" t="s">
+      <c r="F13" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="42"/>
+      <c r="G13" s="34"/>
       <c r="H13" s="22"/>
       <c r="I13" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="J13" s="41" t="s">
+      <c r="J13" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="K13" s="42"/>
+      <c r="K13" s="34"/>
       <c r="L13" s="22"/>
       <c r="M13" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="N13" s="41" t="s">
+      <c r="N13" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="O13" s="42"/>
-    </row>
-    <row r="14" spans="1:15" ht="62.25" customHeight="1">
+      <c r="O13" s="34"/>
+    </row>
+    <row r="14" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="30"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="22"/>
       <c r="E14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="G14" s="30"/>
+      <c r="G14" s="36"/>
       <c r="H14" s="22"/>
       <c r="I14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="29" t="s">
+      <c r="J14" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="K14" s="30"/>
+      <c r="K14" s="36"/>
       <c r="L14" s="22"/>
       <c r="M14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="N14" s="29" t="s">
+      <c r="N14" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="O14" s="30"/>
-    </row>
-    <row r="15" spans="1:15" ht="23.25">
-      <c r="A15" s="39"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="40"/>
+      <c r="O14" s="36"/>
+    </row>
+    <row r="15" spans="1:15" ht="22.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="38"/>
       <c r="D15" s="22"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="40"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="38"/>
       <c r="H15" s="22"/>
       <c r="I15" s="21"/>
-      <c r="J15" s="39" t="s">
+      <c r="J15" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="40"/>
+      <c r="K15" s="38"/>
       <c r="L15" s="22"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
-      <c r="O15" s="40"/>
-    </row>
-    <row r="16" spans="1:15" ht="75.75" customHeight="1">
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="38"/>
+    </row>
+    <row r="16" spans="1:15" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="42"/>
+      <c r="C16" s="34"/>
       <c r="D16" s="22"/>
       <c r="E16" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="41" t="s">
+      <c r="F16" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="42"/>
+      <c r="G16" s="34"/>
       <c r="H16" s="22"/>
       <c r="I16" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="41" t="s">
+      <c r="J16" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="K16" s="42"/>
+      <c r="K16" s="34"/>
       <c r="L16" s="22"/>
       <c r="M16" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="N16" s="41" t="s">
+      <c r="N16" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="O16" s="42"/>
-    </row>
-    <row r="17" spans="1:15" ht="92.25" customHeight="1">
+      <c r="O16" s="34"/>
+    </row>
+    <row r="17" spans="1:15" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="30"/>
+      <c r="C17" s="36"/>
       <c r="D17" s="22"/>
       <c r="E17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="29" t="s">
+      <c r="F17" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="G17" s="30"/>
+      <c r="G17" s="36"/>
       <c r="H17" s="22"/>
       <c r="I17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="J17" s="29" t="s">
+      <c r="J17" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="K17" s="30"/>
+      <c r="K17" s="36"/>
       <c r="L17" s="22"/>
       <c r="M17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="N17" s="29" t="s">
+      <c r="N17" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="O17" s="30"/>
-    </row>
-    <row r="21" spans="1:15" ht="27.75" customHeight="1">
-      <c r="A21" s="33" t="s">
+      <c r="O17" s="36"/>
+    </row>
+    <row r="21" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="34"/>
-    </row>
-    <row r="22" spans="1:15" ht="20.25">
+      <c r="B21" s="41"/>
+      <c r="C21" s="42"/>
+    </row>
+    <row r="22" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A22" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="49"/>
-    </row>
-    <row r="23" spans="1:15" ht="20.25">
+      <c r="C22" s="44"/>
+    </row>
+    <row r="23" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A23" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="49"/>
-    </row>
-    <row r="24" spans="1:15" ht="20.25">
+      <c r="C23" s="44"/>
+    </row>
+    <row r="24" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A24" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="50" t="s">
+      <c r="B24" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="51"/>
-    </row>
-    <row r="25" spans="1:15" s="17" customFormat="1" ht="20.25">
+      <c r="C24" s="50"/>
+    </row>
+    <row r="25" spans="1:15" s="17" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A25" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="35">
+      <c r="B25" s="46">
         <v>45392</v>
       </c>
-      <c r="C25" s="47"/>
-    </row>
-    <row r="26" spans="1:15" ht="20.25">
+      <c r="C25" s="51"/>
+    </row>
+    <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A26" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="48" t="s">
+      <c r="B26" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="49"/>
-    </row>
-    <row r="27" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A27" s="37" t="s">
+      <c r="C26" s="44"/>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="38"/>
-    </row>
-    <row r="28" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A28" s="31" t="s">
+      <c r="B27" s="27"/>
+      <c r="C27" s="28"/>
+    </row>
+    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="32"/>
-    </row>
-    <row r="29" spans="1:15" ht="101.25" customHeight="1">
+      <c r="B28" s="39"/>
+      <c r="C28" s="40"/>
+    </row>
+    <row r="29" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="28"/>
-    </row>
-    <row r="30" spans="1:15" ht="110.25" customHeight="1">
+      <c r="C29" s="49"/>
+    </row>
+    <row r="30" spans="1:15" ht="110.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="30"/>
-    </row>
-    <row r="31" spans="1:15" ht="23.25">
-      <c r="A31" s="31" t="s">
+      <c r="C30" s="36"/>
+    </row>
+    <row r="31" spans="1:15" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A31" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="32"/>
-    </row>
-    <row r="32" spans="1:15" ht="99.75" customHeight="1">
+      <c r="B31" s="39"/>
+      <c r="C31" s="40"/>
+    </row>
+    <row r="32" spans="1:15" ht="99.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="28"/>
-    </row>
-    <row r="33" spans="1:3" ht="56.25" customHeight="1">
+      <c r="C32" s="49"/>
+    </row>
+    <row r="33" spans="1:3" ht="56.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="30"/>
-    </row>
-    <row r="34" spans="1:3" ht="23.25">
-      <c r="A34" s="31" t="s">
+      <c r="C33" s="36"/>
+    </row>
+    <row r="34" spans="1:3" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A34" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="32"/>
-    </row>
-    <row r="35" spans="1:3" ht="94.5" customHeight="1">
+      <c r="B34" s="39"/>
+      <c r="C34" s="40"/>
+    </row>
+    <row r="35" spans="1:3" ht="94.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="28"/>
-    </row>
-    <row r="36" spans="1:3" ht="72" customHeight="1">
+      <c r="C35" s="49"/>
+    </row>
+    <row r="36" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="29" t="s">
+      <c r="B36" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="30"/>
-    </row>
-    <row r="38" spans="1:3" ht="15.75">
+      <c r="C36" s="36"/>
+    </row>
+    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="A34:C34"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="F17:G17"/>
@@ -2573,14 +2540,46 @@
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="A27:C27"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="M1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2594,45 +2593,45 @@
       <selection sqref="A1:K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
-    <col min="2" max="2" width="100.7109375" customWidth="1"/>
-    <col min="3" max="3" width="70.7109375" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" customWidth="1"/>
-    <col min="6" max="6" width="100.7109375" customWidth="1"/>
-    <col min="7" max="7" width="70.7109375" customWidth="1"/>
-    <col min="9" max="9" width="28.28515625" customWidth="1"/>
-    <col min="10" max="10" width="100.7109375" customWidth="1"/>
-    <col min="11" max="11" width="70.7109375" customWidth="1"/>
-    <col min="13" max="13" width="28.28515625" customWidth="1"/>
-    <col min="14" max="14" width="100.7109375" customWidth="1"/>
-    <col min="15" max="15" width="70.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" customWidth="1"/>
+    <col min="3" max="3" width="70.6640625" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="100.6640625" customWidth="1"/>
+    <col min="7" max="7" width="70.6640625" customWidth="1"/>
+    <col min="9" max="9" width="28.33203125" customWidth="1"/>
+    <col min="10" max="10" width="100.6640625" customWidth="1"/>
+    <col min="11" max="11" width="70.6640625" customWidth="1"/>
+    <col min="13" max="13" width="28.33203125" customWidth="1"/>
+    <col min="14" max="14" width="100.6640625" customWidth="1"/>
+    <col min="15" max="15" width="70.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="27.75" customHeight="1">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="46"/>
-      <c r="E1" s="45" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="30"/>
+      <c r="E1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="45"/>
-      <c r="G1" s="46"/>
-      <c r="I1" s="45" t="s">
+      <c r="F1" s="29"/>
+      <c r="G1" s="30"/>
+      <c r="I1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="45"/>
-      <c r="K1" s="46"/>
-      <c r="M1" s="45" t="s">
+      <c r="J1" s="29"/>
+      <c r="K1" s="30"/>
+      <c r="M1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="N1" s="45"/>
-      <c r="O1" s="46"/>
-    </row>
-    <row r="2" spans="1:15" ht="20.25">
+      <c r="N1" s="29"/>
+      <c r="O1" s="30"/>
+    </row>
+    <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
@@ -2662,7 +2661,7 @@
       </c>
       <c r="O2" s="24"/>
     </row>
-    <row r="3" spans="1:15" ht="20.25">
+    <row r="3" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="15" t="s">
         <v>3</v>
       </c>
@@ -2692,7 +2691,7 @@
       </c>
       <c r="O3" s="24"/>
     </row>
-    <row r="4" spans="1:15" ht="20.25">
+    <row r="4" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A4" s="15" t="s">
         <v>5</v>
       </c>
@@ -2722,7 +2721,7 @@
       </c>
       <c r="O4" s="24"/>
     </row>
-    <row r="5" spans="1:15" ht="20.25">
+    <row r="5" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
         <v>10</v>
       </c>
@@ -2752,7 +2751,7 @@
       </c>
       <c r="O5" s="24"/>
     </row>
-    <row r="6" spans="1:15" s="17" customFormat="1" ht="20.25">
+    <row r="6" spans="1:15" s="17" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A6" s="16" t="s">
         <v>12</v>
       </c>
@@ -2782,7 +2781,7 @@
       </c>
       <c r="O6" s="26"/>
     </row>
-    <row r="7" spans="1:15" ht="20.25">
+    <row r="7" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
@@ -2812,417 +2811,417 @@
       </c>
       <c r="O7" s="24"/>
     </row>
-    <row r="8" spans="1:15" ht="15.6" customHeight="1">
-      <c r="A8" s="37" t="s">
+    <row r="8" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="38"/>
-      <c r="E8" s="37" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="28"/>
+      <c r="E8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="38"/>
-      <c r="I8" s="37" t="s">
+      <c r="F8" s="27"/>
+      <c r="G8" s="28"/>
+      <c r="I8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="37"/>
-      <c r="K8" s="38"/>
-      <c r="M8" s="37" t="s">
+      <c r="J8" s="27"/>
+      <c r="K8" s="28"/>
+      <c r="M8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="37"/>
-      <c r="O8" s="38"/>
-    </row>
-    <row r="9" spans="1:15" ht="23.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="44"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="44"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="44"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="43"/>
-      <c r="O9" s="44"/>
-    </row>
-    <row r="10" spans="1:15" ht="105.75" customHeight="1">
+      <c r="N8" s="27"/>
+      <c r="O8" s="28"/>
+    </row>
+    <row r="9" spans="1:15" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="32"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="32"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="32"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="32"/>
+    </row>
+    <row r="10" spans="1:15" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="42"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="22"/>
       <c r="E10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="41" t="s">
+      <c r="F10" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="42"/>
+      <c r="G10" s="34"/>
       <c r="H10" s="22"/>
       <c r="I10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="41" t="s">
+      <c r="J10" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="42"/>
+      <c r="K10" s="34"/>
       <c r="L10" s="22"/>
       <c r="M10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="N10" s="41" t="s">
+      <c r="N10" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="O10" s="42"/>
-    </row>
-    <row r="11" spans="1:15" ht="134.25" customHeight="1">
+      <c r="O10" s="34"/>
+    </row>
+    <row r="11" spans="1:15" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="30"/>
+      <c r="C11" s="36"/>
       <c r="D11" s="22"/>
       <c r="E11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="30"/>
+      <c r="G11" s="36"/>
       <c r="H11" s="22"/>
       <c r="I11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="29" t="s">
+      <c r="J11" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="K11" s="30"/>
+      <c r="K11" s="36"/>
       <c r="L11" s="22"/>
       <c r="M11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="29" t="s">
+      <c r="N11" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="O11" s="30"/>
-    </row>
-    <row r="12" spans="1:15" ht="23.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="40"/>
+      <c r="O11" s="36"/>
+    </row>
+    <row r="12" spans="1:15" ht="22.8" x14ac:dyDescent="0.25">
+      <c r="A12" s="37"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="22"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="40"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="38"/>
       <c r="H12" s="22"/>
       <c r="I12" s="21"/>
-      <c r="J12" s="39" t="s">
+      <c r="J12" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="40"/>
+      <c r="K12" s="38"/>
       <c r="L12" s="22"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="40"/>
-    </row>
-    <row r="13" spans="1:15" ht="96.75" customHeight="1">
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="38"/>
+    </row>
+    <row r="13" spans="1:15" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="42"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="22"/>
       <c r="E13" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="41" t="s">
+      <c r="F13" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="42"/>
+      <c r="G13" s="34"/>
       <c r="H13" s="22"/>
       <c r="I13" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="J13" s="41" t="s">
+      <c r="J13" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="K13" s="42"/>
+      <c r="K13" s="34"/>
       <c r="L13" s="22"/>
       <c r="M13" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="N13" s="41" t="s">
+      <c r="N13" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="O13" s="42"/>
-    </row>
-    <row r="14" spans="1:15" ht="62.25" customHeight="1">
+      <c r="O13" s="34"/>
+    </row>
+    <row r="14" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="30"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="22"/>
       <c r="E14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="G14" s="30"/>
+      <c r="G14" s="36"/>
       <c r="H14" s="22"/>
       <c r="I14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="29" t="s">
+      <c r="J14" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="K14" s="30"/>
+      <c r="K14" s="36"/>
       <c r="L14" s="22"/>
       <c r="M14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="N14" s="29" t="s">
+      <c r="N14" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="O14" s="30"/>
-    </row>
-    <row r="15" spans="1:15" ht="23.25">
-      <c r="A15" s="39"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="40"/>
+      <c r="O14" s="36"/>
+    </row>
+    <row r="15" spans="1:15" ht="22.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="38"/>
       <c r="D15" s="22"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="40"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="38"/>
       <c r="H15" s="22"/>
       <c r="I15" s="21"/>
-      <c r="J15" s="39" t="s">
+      <c r="J15" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="40"/>
+      <c r="K15" s="38"/>
       <c r="L15" s="22"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
-      <c r="O15" s="40"/>
-    </row>
-    <row r="16" spans="1:15" ht="75.75" customHeight="1">
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="38"/>
+    </row>
+    <row r="16" spans="1:15" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="42"/>
+      <c r="C16" s="34"/>
       <c r="D16" s="22"/>
       <c r="E16" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="41" t="s">
+      <c r="F16" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="42"/>
+      <c r="G16" s="34"/>
       <c r="H16" s="22"/>
       <c r="I16" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="41" t="s">
+      <c r="J16" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="K16" s="42"/>
+      <c r="K16" s="34"/>
       <c r="L16" s="22"/>
       <c r="M16" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="N16" s="41" t="s">
+      <c r="N16" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="O16" s="42"/>
-    </row>
-    <row r="17" spans="1:15" ht="92.25" customHeight="1">
+      <c r="O16" s="34"/>
+    </row>
+    <row r="17" spans="1:15" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="30"/>
+      <c r="C17" s="36"/>
       <c r="D17" s="22"/>
       <c r="E17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="29" t="s">
+      <c r="F17" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="G17" s="30"/>
+      <c r="G17" s="36"/>
       <c r="H17" s="22"/>
       <c r="I17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="J17" s="29" t="s">
+      <c r="J17" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="K17" s="30"/>
+      <c r="K17" s="36"/>
       <c r="L17" s="22"/>
       <c r="M17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="N17" s="29" t="s">
+      <c r="N17" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="O17" s="30"/>
-    </row>
-    <row r="21" spans="1:15" ht="27.75" customHeight="1">
-      <c r="A21" s="33" t="s">
+      <c r="O17" s="36"/>
+    </row>
+    <row r="21" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="34"/>
-    </row>
-    <row r="22" spans="1:15" ht="20.25">
+      <c r="B21" s="41"/>
+      <c r="C21" s="42"/>
+    </row>
+    <row r="22" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A22" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="49"/>
-    </row>
-    <row r="23" spans="1:15" ht="20.25">
+      <c r="C22" s="44"/>
+    </row>
+    <row r="23" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A23" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="49"/>
-    </row>
-    <row r="24" spans="1:15" ht="20.25">
+      <c r="C23" s="44"/>
+    </row>
+    <row r="24" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A24" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="50" t="s">
+      <c r="B24" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="51"/>
-    </row>
-    <row r="25" spans="1:15" s="17" customFormat="1" ht="20.25">
+      <c r="C24" s="50"/>
+    </row>
+    <row r="25" spans="1:15" s="17" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A25" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="35">
+      <c r="B25" s="46">
         <v>45392</v>
       </c>
-      <c r="C25" s="47"/>
+      <c r="C25" s="51"/>
       <c r="K25"/>
       <c r="L25"/>
       <c r="M25"/>
       <c r="N25"/>
     </row>
-    <row r="26" spans="1:15" ht="20.25">
+    <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A26" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="48" t="s">
+      <c r="B26" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="49"/>
-    </row>
-    <row r="27" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A27" s="37" t="s">
+      <c r="C26" s="44"/>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="38"/>
-    </row>
-    <row r="28" spans="1:15" ht="23.25">
-      <c r="A28" s="31" t="s">
+      <c r="B27" s="27"/>
+      <c r="C27" s="28"/>
+    </row>
+    <row r="28" spans="1:15" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A28" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="32"/>
-    </row>
-    <row r="29" spans="1:15" ht="101.25" customHeight="1">
+      <c r="B28" s="39"/>
+      <c r="C28" s="40"/>
+    </row>
+    <row r="29" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="28"/>
-    </row>
-    <row r="30" spans="1:15" ht="110.25" customHeight="1">
+      <c r="C29" s="49"/>
+    </row>
+    <row r="30" spans="1:15" ht="110.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="C30" s="30"/>
-    </row>
-    <row r="31" spans="1:15" ht="23.25">
-      <c r="A31" s="31" t="s">
+      <c r="C30" s="36"/>
+    </row>
+    <row r="31" spans="1:15" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A31" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="32"/>
-    </row>
-    <row r="32" spans="1:15" ht="99.75" customHeight="1">
+      <c r="B31" s="39"/>
+      <c r="C31" s="40"/>
+    </row>
+    <row r="32" spans="1:15" ht="99.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="28"/>
-    </row>
-    <row r="33" spans="1:3" ht="56.25" customHeight="1">
+      <c r="C32" s="49"/>
+    </row>
+    <row r="33" spans="1:3" ht="56.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="30"/>
-    </row>
-    <row r="34" spans="1:3" ht="23.25">
-      <c r="A34" s="31" t="s">
+      <c r="C33" s="36"/>
+    </row>
+    <row r="34" spans="1:3" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A34" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="32"/>
-    </row>
-    <row r="35" spans="1:3" ht="94.5" customHeight="1">
+      <c r="B34" s="39"/>
+      <c r="C34" s="40"/>
+    </row>
+    <row r="35" spans="1:3" ht="94.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="28"/>
-    </row>
-    <row r="36" spans="1:3" ht="72" customHeight="1">
+      <c r="C35" s="49"/>
+    </row>
+    <row r="36" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="29" t="s">
+      <c r="B36" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="C36" s="30"/>
-    </row>
-    <row r="38" spans="1:3" ht="15.75">
+      <c r="C36" s="36"/>
+    </row>
+    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>48</v>
       </c>
@@ -3230,46 +3229,14 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="A34:C34"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="F17:G17"/>
@@ -3282,14 +3249,46 @@
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="A27:C27"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="M1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3303,45 +3302,45 @@
       <selection sqref="A1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
-    <col min="2" max="2" width="100.7109375" customWidth="1"/>
-    <col min="3" max="3" width="70.7109375" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" customWidth="1"/>
-    <col min="6" max="6" width="100.7109375" customWidth="1"/>
-    <col min="7" max="7" width="70.7109375" customWidth="1"/>
-    <col min="9" max="9" width="28.28515625" customWidth="1"/>
-    <col min="10" max="10" width="100.7109375" customWidth="1"/>
-    <col min="11" max="11" width="70.7109375" customWidth="1"/>
-    <col min="13" max="13" width="28.28515625" customWidth="1"/>
-    <col min="14" max="14" width="100.7109375" customWidth="1"/>
-    <col min="15" max="15" width="70.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" customWidth="1"/>
+    <col min="3" max="3" width="70.6640625" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="100.6640625" customWidth="1"/>
+    <col min="7" max="7" width="70.6640625" customWidth="1"/>
+    <col min="9" max="9" width="28.33203125" customWidth="1"/>
+    <col min="10" max="10" width="100.6640625" customWidth="1"/>
+    <col min="11" max="11" width="70.6640625" customWidth="1"/>
+    <col min="13" max="13" width="28.33203125" customWidth="1"/>
+    <col min="14" max="14" width="100.6640625" customWidth="1"/>
+    <col min="15" max="15" width="70.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="28.35" customHeight="1">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:15" ht="28.35" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="46"/>
-      <c r="E1" s="45" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="30"/>
+      <c r="E1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="45"/>
-      <c r="G1" s="46"/>
-      <c r="I1" s="45" t="s">
+      <c r="F1" s="29"/>
+      <c r="G1" s="30"/>
+      <c r="I1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="45"/>
-      <c r="K1" s="46"/>
-      <c r="M1" s="45" t="s">
+      <c r="J1" s="29"/>
+      <c r="K1" s="30"/>
+      <c r="M1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="N1" s="45"/>
-      <c r="O1" s="46"/>
-    </row>
-    <row r="2" spans="1:15" ht="20.25">
+      <c r="N1" s="29"/>
+      <c r="O1" s="30"/>
+    </row>
+    <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
@@ -3371,7 +3370,7 @@
       </c>
       <c r="O2" s="24"/>
     </row>
-    <row r="3" spans="1:15" ht="20.25">
+    <row r="3" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="15" t="s">
         <v>3</v>
       </c>
@@ -3401,7 +3400,7 @@
       </c>
       <c r="O3" s="24"/>
     </row>
-    <row r="4" spans="1:15" ht="20.25">
+    <row r="4" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A4" s="15" t="s">
         <v>5</v>
       </c>
@@ -3431,7 +3430,7 @@
       </c>
       <c r="O4" s="24"/>
     </row>
-    <row r="5" spans="1:15" ht="20.25">
+    <row r="5" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
         <v>10</v>
       </c>
@@ -3461,7 +3460,7 @@
       </c>
       <c r="O5" s="24"/>
     </row>
-    <row r="6" spans="1:15" s="17" customFormat="1" ht="20.25">
+    <row r="6" spans="1:15" s="17" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A6" s="16" t="s">
         <v>12</v>
       </c>
@@ -3491,7 +3490,7 @@
       </c>
       <c r="O6" s="26"/>
     </row>
-    <row r="7" spans="1:15" ht="20.25">
+    <row r="7" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
@@ -3521,413 +3520,413 @@
       </c>
       <c r="O7" s="24"/>
     </row>
-    <row r="8" spans="1:15" ht="15.6" customHeight="1">
-      <c r="A8" s="37" t="s">
+    <row r="8" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="38"/>
-      <c r="E8" s="37" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="28"/>
+      <c r="E8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="38"/>
-      <c r="I8" s="37" t="s">
+      <c r="F8" s="27"/>
+      <c r="G8" s="28"/>
+      <c r="I8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="37"/>
-      <c r="K8" s="38"/>
-      <c r="M8" s="37" t="s">
+      <c r="J8" s="27"/>
+      <c r="K8" s="28"/>
+      <c r="M8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="37"/>
-      <c r="O8" s="38"/>
-    </row>
-    <row r="9" spans="1:15" ht="23.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="44"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="44"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="44"/>
-      <c r="M9" s="43"/>
-      <c r="N9" s="43"/>
-      <c r="O9" s="44"/>
-    </row>
-    <row r="10" spans="1:15" ht="105.75" customHeight="1">
+      <c r="N8" s="27"/>
+      <c r="O8" s="28"/>
+    </row>
+    <row r="9" spans="1:15" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="32"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="32"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="32"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="32"/>
+    </row>
+    <row r="10" spans="1:15" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="42"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="22"/>
       <c r="E10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="41" t="s">
+      <c r="F10" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="42"/>
+      <c r="G10" s="34"/>
       <c r="H10" s="22"/>
       <c r="I10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="41" t="s">
+      <c r="J10" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="42"/>
+      <c r="K10" s="34"/>
       <c r="L10" s="22"/>
       <c r="M10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="N10" s="41" t="s">
+      <c r="N10" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="O10" s="42"/>
-    </row>
-    <row r="11" spans="1:15" ht="134.25" customHeight="1">
+      <c r="O10" s="34"/>
+    </row>
+    <row r="11" spans="1:15" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="30"/>
+      <c r="C11" s="36"/>
       <c r="D11" s="22"/>
       <c r="E11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="G11" s="30"/>
+      <c r="G11" s="36"/>
       <c r="H11" s="22"/>
       <c r="I11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="29" t="s">
+      <c r="J11" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="K11" s="30"/>
+      <c r="K11" s="36"/>
       <c r="L11" s="22"/>
       <c r="M11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="29" t="s">
+      <c r="N11" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="O11" s="30"/>
-    </row>
-    <row r="12" spans="1:15" ht="23.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="40"/>
+      <c r="O11" s="36"/>
+    </row>
+    <row r="12" spans="1:15" ht="22.8" x14ac:dyDescent="0.25">
+      <c r="A12" s="37"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="22"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="40"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="38"/>
       <c r="H12" s="22"/>
       <c r="I12" s="21"/>
-      <c r="J12" s="39" t="s">
+      <c r="J12" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="40"/>
+      <c r="K12" s="38"/>
       <c r="L12" s="22"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="40"/>
-    </row>
-    <row r="13" spans="1:15" ht="96.75" customHeight="1">
+      <c r="M12" s="37"/>
+      <c r="N12" s="37"/>
+      <c r="O12" s="38"/>
+    </row>
+    <row r="13" spans="1:15" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="42"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="22"/>
       <c r="E13" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="41" t="s">
+      <c r="F13" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="42"/>
+      <c r="G13" s="34"/>
       <c r="H13" s="22"/>
       <c r="I13" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="J13" s="41" t="s">
+      <c r="J13" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="K13" s="42"/>
+      <c r="K13" s="34"/>
       <c r="L13" s="22"/>
       <c r="M13" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="N13" s="41" t="s">
+      <c r="N13" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="O13" s="42"/>
-    </row>
-    <row r="14" spans="1:15" ht="62.25" customHeight="1">
+      <c r="O13" s="34"/>
+    </row>
+    <row r="14" spans="1:15" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="30"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="22"/>
       <c r="E14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="G14" s="30"/>
+      <c r="G14" s="36"/>
       <c r="H14" s="22"/>
       <c r="I14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="29" t="s">
+      <c r="J14" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="K14" s="30"/>
+      <c r="K14" s="36"/>
       <c r="L14" s="22"/>
       <c r="M14" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="N14" s="29" t="s">
+      <c r="N14" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="O14" s="30"/>
-    </row>
-    <row r="15" spans="1:15" ht="23.25">
-      <c r="A15" s="39"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="40"/>
+      <c r="O14" s="36"/>
+    </row>
+    <row r="15" spans="1:15" ht="22.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="38"/>
       <c r="D15" s="22"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="40"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="38"/>
       <c r="H15" s="22"/>
       <c r="I15" s="21"/>
-      <c r="J15" s="39" t="s">
+      <c r="J15" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="40"/>
+      <c r="K15" s="38"/>
       <c r="L15" s="22"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
-      <c r="O15" s="40"/>
-    </row>
-    <row r="16" spans="1:15" ht="75.75" customHeight="1">
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="38"/>
+    </row>
+    <row r="16" spans="1:15" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="42"/>
+      <c r="C16" s="34"/>
       <c r="D16" s="22"/>
       <c r="E16" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="41" t="s">
+      <c r="F16" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="42"/>
+      <c r="G16" s="34"/>
       <c r="H16" s="22"/>
       <c r="I16" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="41" t="s">
+      <c r="J16" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="K16" s="42"/>
+      <c r="K16" s="34"/>
       <c r="L16" s="22"/>
       <c r="M16" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="N16" s="41" t="s">
+      <c r="N16" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="O16" s="42"/>
-    </row>
-    <row r="17" spans="1:15" ht="92.25" customHeight="1">
+      <c r="O16" s="34"/>
+    </row>
+    <row r="17" spans="1:15" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="C17" s="30"/>
+      <c r="C17" s="36"/>
       <c r="D17" s="22"/>
       <c r="E17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="29" t="s">
+      <c r="F17" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="G17" s="30"/>
+      <c r="G17" s="36"/>
       <c r="H17" s="22"/>
       <c r="I17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="J17" s="29" t="s">
+      <c r="J17" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="K17" s="30"/>
+      <c r="K17" s="36"/>
       <c r="L17" s="22"/>
       <c r="M17" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="N17" s="29" t="s">
+      <c r="N17" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="O17" s="30"/>
-    </row>
-    <row r="21" spans="1:15" ht="27.75" customHeight="1">
-      <c r="A21" s="33" t="s">
+      <c r="O17" s="36"/>
+    </row>
+    <row r="21" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="34"/>
-    </row>
-    <row r="22" spans="1:15" ht="20.25">
+      <c r="B21" s="41"/>
+      <c r="C21" s="42"/>
+    </row>
+    <row r="22" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A22" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="49"/>
-    </row>
-    <row r="23" spans="1:15" ht="20.25">
+      <c r="C22" s="44"/>
+    </row>
+    <row r="23" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A23" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="49"/>
-    </row>
-    <row r="24" spans="1:15" ht="20.25">
+      <c r="C23" s="44"/>
+    </row>
+    <row r="24" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A24" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="50" t="s">
+      <c r="B24" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="51"/>
-    </row>
-    <row r="25" spans="1:15" s="17" customFormat="1" ht="20.25">
+      <c r="C24" s="50"/>
+    </row>
+    <row r="25" spans="1:15" s="17" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A25" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="35">
+      <c r="B25" s="46">
         <v>45392</v>
       </c>
-      <c r="C25" s="47"/>
-    </row>
-    <row r="26" spans="1:15" ht="20.25">
+      <c r="C25" s="51"/>
+    </row>
+    <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A26" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="48" t="s">
+      <c r="B26" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="49"/>
-    </row>
-    <row r="27" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A27" s="37" t="s">
+      <c r="C26" s="44"/>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="38"/>
-    </row>
-    <row r="28" spans="1:15" ht="23.25">
-      <c r="A28" s="31" t="s">
+      <c r="B27" s="27"/>
+      <c r="C27" s="28"/>
+    </row>
+    <row r="28" spans="1:15" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A28" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="32"/>
-    </row>
-    <row r="29" spans="1:15" ht="101.25" customHeight="1">
+      <c r="B28" s="39"/>
+      <c r="C28" s="40"/>
+    </row>
+    <row r="29" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="28"/>
-    </row>
-    <row r="30" spans="1:15" ht="110.25" customHeight="1">
+      <c r="C29" s="49"/>
+    </row>
+    <row r="30" spans="1:15" ht="110.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="30"/>
-    </row>
-    <row r="31" spans="1:15" ht="23.25">
-      <c r="A31" s="31" t="s">
+      <c r="C30" s="36"/>
+    </row>
+    <row r="31" spans="1:15" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A31" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="32"/>
-    </row>
-    <row r="32" spans="1:15" ht="99.75" customHeight="1">
+      <c r="B31" s="39"/>
+      <c r="C31" s="40"/>
+    </row>
+    <row r="32" spans="1:15" ht="99.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="28"/>
-    </row>
-    <row r="33" spans="1:3" ht="56.25" customHeight="1">
+      <c r="C32" s="49"/>
+    </row>
+    <row r="33" spans="1:3" ht="56.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="29" t="s">
+      <c r="B33" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="C33" s="30"/>
-    </row>
-    <row r="34" spans="1:3" ht="23.25">
-      <c r="A34" s="31" t="s">
+      <c r="C33" s="36"/>
+    </row>
+    <row r="34" spans="1:3" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A34" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="32"/>
-    </row>
-    <row r="35" spans="1:3" ht="94.5" customHeight="1">
+      <c r="B34" s="39"/>
+      <c r="C34" s="40"/>
+    </row>
+    <row r="35" spans="1:3" ht="94.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="28"/>
-    </row>
-    <row r="36" spans="1:3" ht="72" customHeight="1">
+      <c r="C35" s="49"/>
+    </row>
+    <row r="36" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="29" t="s">
+      <c r="B36" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="C36" s="30"/>
-    </row>
-    <row r="38" spans="1:3" ht="15.75">
+      <c r="C36" s="36"/>
+    </row>
+    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>48</v>
       </c>
@@ -3935,46 +3934,14 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="A34:C34"/>
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="F17:G17"/>
@@ -3987,704 +3954,215 @@
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="A27:C27"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="M1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C593B2B-509F-4EE1-8616-C472E741EF17}">
-  <dimension ref="A1:O38"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
-    <col min="2" max="2" width="100.7109375" customWidth="1"/>
-    <col min="3" max="3" width="70.7109375" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" customWidth="1"/>
-    <col min="6" max="6" width="100.7109375" customWidth="1"/>
-    <col min="7" max="7" width="70.7109375" customWidth="1"/>
-    <col min="9" max="9" width="28.28515625" customWidth="1"/>
-    <col min="10" max="10" width="100.7109375" customWidth="1"/>
-    <col min="11" max="11" width="70.7109375" customWidth="1"/>
-    <col min="13" max="13" width="28.28515625" customWidth="1"/>
-    <col min="14" max="14" width="100.7109375" customWidth="1"/>
-    <col min="15" max="15" width="70.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" ht="28.35" customHeight="1">
-      <c r="A1" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="46"/>
-      <c r="E1" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="45"/>
-      <c r="G1" s="46"/>
-      <c r="I1" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="45"/>
-      <c r="K1" s="46"/>
-    </row>
-    <row r="2" spans="1:15" ht="20.25">
-      <c r="A2" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="24"/>
-      <c r="E2" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="23"/>
-      <c r="G2" s="24"/>
-      <c r="I2" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="23"/>
-      <c r="K2" s="24"/>
-    </row>
-    <row r="3" spans="1:15" ht="20.25">
-      <c r="A3" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="24"/>
-      <c r="E3" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="24"/>
-      <c r="I3" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="23"/>
-      <c r="K3" s="24"/>
-    </row>
-    <row r="4" spans="1:15" ht="20.25">
-      <c r="A4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="24"/>
-      <c r="E4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24"/>
-      <c r="I4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" s="23"/>
-      <c r="K4" s="24"/>
-    </row>
-    <row r="5" spans="1:15" ht="20.25">
-      <c r="A5" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="24"/>
-      <c r="E5" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="24"/>
-      <c r="I5" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="23"/>
-      <c r="K5" s="24"/>
-    </row>
-    <row r="6" spans="1:15" s="17" customFormat="1" ht="20.25">
-      <c r="A6" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="26"/>
-      <c r="E6" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="26"/>
-      <c r="I6" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="25"/>
-      <c r="K6" s="26"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-      <c r="O6"/>
-    </row>
-    <row r="7" spans="1:15" ht="20.25">
-      <c r="A7" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="24"/>
-      <c r="E7" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="24"/>
-      <c r="I7" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="23"/>
-      <c r="K7" s="24"/>
-    </row>
-    <row r="8" spans="1:15" ht="15.6" customHeight="1">
-      <c r="A8" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="38"/>
-      <c r="E8" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="38"/>
-      <c r="I8" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="37"/>
-      <c r="K8" s="38"/>
-    </row>
-    <row r="9" spans="1:15" ht="23.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="44"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="44"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="44"/>
-    </row>
-    <row r="10" spans="1:15" ht="105.75" customHeight="1">
-      <c r="A10" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="42"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="K10" s="42"/>
-    </row>
-    <row r="11" spans="1:15" ht="134.25" customHeight="1">
-      <c r="A11" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="29"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="29"/>
-      <c r="K11" s="30"/>
-    </row>
-    <row r="12" spans="1:15" ht="23.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="40"/>
-    </row>
-    <row r="13" spans="1:15" ht="96.75" customHeight="1">
-      <c r="A13" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="42"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="K13" s="42"/>
-    </row>
-    <row r="14" spans="1:15" ht="62.25" customHeight="1">
-      <c r="A14" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="29"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="29"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" s="29"/>
-      <c r="K14" s="30"/>
-    </row>
-    <row r="15" spans="1:15" ht="23.25">
-      <c r="A15" s="39"/>
-      <c r="B15" s="39"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="K15" s="40"/>
-    </row>
-    <row r="16" spans="1:15" ht="75.75" customHeight="1">
-      <c r="A16" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="42"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="J16" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="K16" s="42"/>
-    </row>
-    <row r="17" spans="1:15" ht="92.25" customHeight="1">
-      <c r="A17" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="F17" s="29"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" s="29"/>
-      <c r="K17" s="30"/>
-    </row>
-    <row r="21" spans="1:15" ht="27.75">
-      <c r="A21" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="34"/>
-    </row>
-    <row r="22" spans="1:15" ht="20.25">
-      <c r="A22" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="48"/>
-      <c r="C22" s="49"/>
-    </row>
-    <row r="23" spans="1:15" ht="20.25">
-      <c r="A23" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="48"/>
-      <c r="C23" s="49"/>
-    </row>
-    <row r="24" spans="1:15" ht="20.25">
-      <c r="A24" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="50"/>
-      <c r="C24" s="49"/>
-    </row>
-    <row r="25" spans="1:15" s="17" customFormat="1" ht="20.25">
-      <c r="A25" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="36"/>
-      <c r="L25"/>
-      <c r="M25"/>
-      <c r="N25"/>
-      <c r="O25"/>
-    </row>
-    <row r="26" spans="1:15" ht="20.25">
-      <c r="A26" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="48"/>
-      <c r="C26" s="49"/>
-    </row>
-    <row r="27" spans="1:15" ht="15.75">
-      <c r="A27" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="38"/>
-    </row>
-    <row r="28" spans="1:15" ht="23.25">
-      <c r="A28" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="32"/>
-    </row>
-    <row r="29" spans="1:15" ht="101.25" customHeight="1">
-      <c r="A29" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="C29" s="28"/>
-    </row>
-    <row r="30" spans="1:15" ht="110.25" customHeight="1">
-      <c r="A30" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="29"/>
-      <c r="C30" s="30"/>
-    </row>
-    <row r="31" spans="1:15" ht="23.25">
-      <c r="A31" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="32"/>
-    </row>
-    <row r="32" spans="1:15" ht="99.75" customHeight="1">
-      <c r="A32" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" s="28"/>
-    </row>
-    <row r="33" spans="1:3" ht="68.099999999999994" customHeight="1">
-      <c r="A33" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33" s="29"/>
-      <c r="C33" s="30"/>
-    </row>
-    <row r="34" spans="1:3" ht="23.25">
-      <c r="A34" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="32"/>
-    </row>
-    <row r="35" spans="1:3" ht="94.5" customHeight="1">
-      <c r="A35" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="28"/>
-    </row>
-    <row r="36" spans="1:3" ht="72" customHeight="1">
-      <c r="A36" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="29"/>
-      <c r="C36" s="30"/>
-    </row>
-    <row r="38" spans="1:3" ht="15.75">
-      <c r="A38" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38" s="19"/>
-    </row>
-  </sheetData>
-  <mergeCells count="49">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="F17:G17"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="4" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" zoomScale="68" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="68" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="198.42578125" customWidth="1"/>
+    <col min="1" max="1" width="198.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="39.950000000000003" customHeight="1">
+    <row r="1" spans="1:4" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" ht="31.5">
+    <row r="3" spans="1:4" s="3" customFormat="1" ht="31.2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>98</v>
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" ht="27.75" customHeight="1">
+    <row r="4" spans="1:4" s="3" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>99</v>
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="5" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>100</v>
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="6" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>101</v>
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
+    <row r="7" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>102</v>
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="8" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
     </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" ht="73.5" customHeight="1">
+    <row r="9" spans="1:4" s="2" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="10" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="11" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="12" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="13" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="14" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="15" spans="1:4" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
     </row>
-    <row r="16" spans="1:4" s="2" customFormat="1" ht="44.25" customHeight="1">
+    <row r="16" spans="1:4" s="2" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="17" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="18" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="19" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:1" s="2" customFormat="1" ht="35.25" customHeight="1">
+    <row r="20" spans="1:1" s="2" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="21" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
     </row>
-    <row r="22" spans="1:1" s="2" customFormat="1" ht="48.75" customHeight="1">
+    <row r="22" spans="1:1" s="2" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="23" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="24" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="25" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="26" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
     </row>
-    <row r="27" spans="1:1" s="2" customFormat="1" ht="46.5" customHeight="1">
+    <row r="27" spans="1:1" s="2" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="28" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="29" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="30" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1">
+    <row r="31" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>122</v>
       </c>
@@ -4840,6 +4318,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -4848,20 +4332,37 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8535C7D-FF6F-43CC-8BB8-3EA5141E1CDB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C8535C7D-FF6F-43CC-8BB8-3EA5141E1CDB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="63b2c1dc-91a4-4475-a664-303126d4a333"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3317C67C-DFC0-407D-B7A5-E63D73EC344A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BCDA050-3553-4C0B-BF90-4BE0C31B84AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BCDA050-3553-4C0B-BF90-4BE0C31B84AD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3317C67C-DFC0-407D-B7A5-E63D73EC344A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>